<commit_message>
added exporting and importing to csv
</commit_message>
<xml_diff>
--- a/plan.xlsx
+++ b/plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7c610102d569593a/Documents/Dungeons and Dragons/Monster Generator/MonsterMaker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{F7BAC580-E558-44D3-8B94-E11F5B16BD49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D8349EA8-F103-4669-856B-C3B594462FC2}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="8_{F7BAC580-E558-44D3-8B94-E11F5B16BD49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C1D46141-00EC-4D80-B0C7-22DE1FC80657}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CA161434-59EF-4258-8AA4-77EC92F51F91}"/>
+    <workbookView xWindow="2295" yWindow="2295" windowWidth="21600" windowHeight="11295" xr2:uid="{CA161434-59EF-4258-8AA4-77EC92F51F91}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>task</t>
   </si>
@@ -54,6 +54,18 @@
   </si>
   <si>
     <t>not started</t>
+  </si>
+  <si>
+    <t>make monster abilties</t>
+  </si>
+  <si>
+    <t>make monster attacks</t>
+  </si>
+  <si>
+    <t>make CR calculator</t>
+  </si>
+  <si>
+    <t>finished?</t>
   </si>
 </sst>
 </file>
@@ -106,6 +118,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -405,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8305BBA-4708-4D81-B756-0EDE944CBE66}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -435,10 +451,34 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>